<commit_message>
Updated the Development Log
</commit_message>
<xml_diff>
--- a/Development Log.xlsx
+++ b/Development Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashtaga\P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashtaga\P1\CSCE315Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4141FE0-F146-4B12-B525-E48F8B91D558}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F47794-3D8D-4620-A218-DF8EEC061363}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E078DCC-6A95-4A08-AE00-36DAE6A9C2D0}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
-  <si>
-    <t>???</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Set up the ANTLR4 listener (phase 2, step 2, part 1)</t>
+  </si>
+  <si>
+    <t>Worked to understand what we need to do to complete phase 2</t>
   </si>
 </sst>
 </file>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9618D4EA-B1AA-4118-89F0-E4BEFF2F685F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,30 +432,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43733</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" s="2">
+        <v>0.375</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -466,10 +466,10 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -480,10 +480,10 @@
         <v>0.625</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,24 +494,32 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43736</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
+      <c r="B6" s="2">
+        <v>0.85416666666666663</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43737</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merged everything into master
</commit_message>
<xml_diff>
--- a/Development Log.xlsx
+++ b/Development Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Made the input consistent with the grammar we have (i.e. normalizing the input) - project is ready for submission</t>
+  </si>
+  <si>
+    <t>Merged branches back to master</t>
   </si>
 </sst>
 </file>
@@ -167,16 +170,13 @@
       <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="10.0"/>
     </font>
     <font/>
   </fonts>
@@ -214,47 +214,41 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -889,13 +883,13 @@
       <c r="A30" s="11">
         <v>43753.0</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <v>0.6666666666666666</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -903,13 +897,13 @@
       <c r="A31" s="11">
         <v>43755.0</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="10">
         <v>0.4583333333333333</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -917,13 +911,13 @@
       <c r="A32" s="11">
         <v>43755.0</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="10">
         <v>0.7083333333333334</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -931,13 +925,13 @@
       <c r="A33" s="11">
         <v>43755.0</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="10">
         <v>0.7708333333333334</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -945,14 +939,28 @@
       <c r="A34" s="11">
         <v>43755.0</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="10">
         <v>0.8541666666666666</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="9" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="11">
+        <v>43756.0</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>